<commit_message>
HIKER-M Upate Pairing Matrix and Attendence List [TV]
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viktoriatrummer/Library/Mobile Documents/com~apple~CloudDocs/Uni/SS21/SoftwareTechnology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viktoriatrummer/Desktop/Uni/Master/gitRepos/Team_28/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123FB496-C0A3-2C42-B293-90C9AE11DD34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131C8AD0-1142-5741-9B4E-DFFFDA8FFECF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="37360" windowHeight="19540" xr2:uid="{DA1D2984-0AA3-DF42-B2E6-F1E655DF0FBC}"/>
+    <workbookView xWindow="17020" yWindow="620" windowWidth="37360" windowHeight="19540" xr2:uid="{DA1D2984-0AA3-DF42-B2E6-F1E655DF0FBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="13">
   <si>
     <t>Feldgrill, Lukas André</t>
   </si>
@@ -79,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,6 +107,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -128,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -144,6 +151,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,7 +472,7 @@
   <dimension ref="C2:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -486,6 +496,9 @@
       <c r="F4" s="3">
         <v>44307</v>
       </c>
+      <c r="G4" s="3">
+        <v>44314</v>
+      </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
@@ -500,7 +513,9 @@
       <c r="F5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -515,6 +530,9 @@
       <c r="F6" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
@@ -529,6 +547,9 @@
       <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G7" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
@@ -543,6 +564,9 @@
       <c r="F8" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G8" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
@@ -557,6 +581,9 @@
       <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G9" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
@@ -571,6 +598,9 @@
       <c r="F10" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G10" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
@@ -585,6 +615,9 @@
       <c r="F11" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G11" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
@@ -599,6 +632,9 @@
       <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G12" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
@@ -613,6 +649,9 @@
       <c r="F13" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G13" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
@@ -627,6 +666,9 @@
       <c r="F14" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G14" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
@@ -639,6 +681,9 @@
         <v>12</v>
       </c>
       <c r="F15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
HIKER-M Update Pairing Matrix and Attendacne List[TV]
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viktoriatrummer/Desktop/Uni/Master/gitRepos/Team_28/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09263A0-C899-7B47-96C7-052AB94EC55B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EFC668-F2B2-1B48-99BA-4B0F47A04D81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="520" windowWidth="37360" windowHeight="19540" xr2:uid="{DA1D2984-0AA3-DF42-B2E6-F1E655DF0FBC}"/>
+    <workbookView xWindow="6360" yWindow="500" windowWidth="32040" windowHeight="19540" xr2:uid="{DA1D2984-0AA3-DF42-B2E6-F1E655DF0FBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="14">
   <si>
     <t>Feldgrill, Lukas André</t>
   </si>
@@ -472,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB470405-F039-FE48-B3FC-DF8049F8FB45}">
-  <dimension ref="C2:H15"/>
+  <dimension ref="C2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -484,12 +484,12 @@
     <col min="4" max="4" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:10" ht="21" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="D4" s="3">
         <v>44279</v>
       </c>
@@ -505,8 +505,11 @@
       <c r="H4" s="3">
         <v>44321</v>
       </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="3">
+        <v>44328</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,8 +528,11 @@
       <c r="H5" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
@@ -545,8 +551,11 @@
       <c r="H6" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
@@ -565,8 +574,11 @@
       <c r="H7" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
@@ -585,8 +597,11 @@
       <c r="H8" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
@@ -605,8 +620,11 @@
       <c r="H9" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
@@ -625,8 +643,11 @@
       <c r="H10" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
@@ -645,8 +666,11 @@
       <c r="H11" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
@@ -665,8 +689,11 @@
       <c r="H12" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
@@ -685,8 +712,11 @@
       <c r="H13" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
@@ -705,8 +735,12 @@
       <c r="H14" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
@@ -723,6 +757,9 @@
         <v>12</v>
       </c>
       <c r="H15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
HIKER-M Update Attendance List[TV]
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viktoriatrummer/Desktop/Uni/Master/gitRepos/Team_28/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EFC668-F2B2-1B48-99BA-4B0F47A04D81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF53F450-4D4F-ED4A-B989-D9F6BF8FA856}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6360" yWindow="500" windowWidth="32040" windowHeight="19540" xr2:uid="{DA1D2984-0AA3-DF42-B2E6-F1E655DF0FBC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="15">
   <si>
     <t>Feldgrill, Lukas André</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>✓ (left at 16:30)</t>
   </si>
 </sst>
 </file>
@@ -475,13 +478,14 @@
   <dimension ref="C2:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="38.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="4"/>
+    <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="21" x14ac:dyDescent="0.25">
@@ -508,6 +512,9 @@
       <c r="I4" s="3">
         <v>44328</v>
       </c>
+      <c r="J4" s="3">
+        <v>44335</v>
+      </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
@@ -531,6 +538,9 @@
       <c r="I5" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -554,6 +564,9 @@
       <c r="I6" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J6" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
@@ -577,6 +590,9 @@
       <c r="I7" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J7" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
@@ -600,6 +616,9 @@
       <c r="I8" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J8" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
@@ -621,6 +640,9 @@
         <v>12</v>
       </c>
       <c r="I9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -646,6 +668,9 @@
       <c r="I10" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J10" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
@@ -669,6 +694,9 @@
       <c r="I11" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J11" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
@@ -692,6 +720,9 @@
       <c r="I12" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J12" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
@@ -715,6 +746,9 @@
       <c r="I13" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="J13" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
@@ -738,7 +772,9 @@
       <c r="I14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="4"/>
+      <c r="J14" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
@@ -760,6 +796,9 @@
         <v>12</v>
       </c>
       <c r="I15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
HIKER-M Update Attendance List [TV]
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viktoriatrummer/Desktop/Uni/Master/gitRepos/Team_28/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BAE3DF-93E9-8645-8B36-3566AF301CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D6E073-E569-5348-81E6-C1B779801B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="500" windowWidth="32040" windowHeight="19540" xr2:uid="{DA1D2984-0AA3-DF42-B2E6-F1E655DF0FBC}"/>
+    <workbookView xWindow="6580" yWindow="500" windowWidth="31720" windowHeight="19560" xr2:uid="{DA1D2984-0AA3-DF42-B2E6-F1E655DF0FBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="16">
   <si>
     <t>Feldgrill, Lukas André</t>
   </si>
@@ -75,10 +75,13 @@
     <t>✓</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>✓ (left at 16:30)</t>
+  </si>
+  <si>
+    <t>✘</t>
+  </si>
+  <si>
+    <t>✓ (Joined at 14:30)</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB470405-F039-FE48-B3FC-DF8049F8FB45}">
-  <dimension ref="C2:K15"/>
+  <dimension ref="C2:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -486,14 +489,15 @@
     <col min="3" max="3" width="38.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="4"/>
     <col min="9" max="9" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:12" ht="21" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D4" s="3">
         <v>44279</v>
       </c>
@@ -518,8 +522,11 @@
       <c r="K4" s="3">
         <v>44342</v>
       </c>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="3">
+        <v>44349</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
@@ -547,8 +554,11 @@
       <c r="K5" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
@@ -576,8 +586,11 @@
       <c r="K6" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
@@ -605,8 +618,11 @@
       <c r="K7" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
@@ -623,7 +639,7 @@
         <v>12</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>12</v>
@@ -634,8 +650,11 @@
       <c r="K8" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
@@ -655,7 +674,7 @@
         <v>12</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>12</v>
@@ -663,8 +682,11 @@
       <c r="K9" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
@@ -692,8 +714,11 @@
       <c r="K10" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
@@ -721,8 +746,11 @@
       <c r="K11" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
@@ -750,8 +778,11 @@
       <c r="K12" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
@@ -779,8 +810,11 @@
       <c r="K13" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
@@ -797,7 +831,7 @@
         <v>12</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>12</v>
@@ -808,8 +842,11 @@
       <c r="K14" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>10</v>
       </c>
@@ -835,6 +872,9 @@
         <v>12</v>
       </c>
       <c r="K15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>